<commit_message>
Updated excell data and added clear browser data fuction and clear recent app
</commit_message>
<xml_diff>
--- a/Resources/GoogleMapTestData.xlsx
+++ b/Resources/GoogleMapTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyanadeep Sahoo\eclipse-workspace\2nd_Phone_RECONRestorationReconstructionLLC_RepairFireDamage\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gyanadeep Sahoo\eclipse-workspace\2nd_Phone_CreativeHomeImprovementLLC_WindowsReplacement\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4B20C8-A514-4DE2-8A7F-84D8D0287815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC048A18-BDC4-4574-A653-31EA9B9D5A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="7" xr2:uid="{273AC0EA-EF08-44F8-A0C8-9FE87C213ADF}"/>
+    <workbookView xWindow="4380" yWindow="2295" windowWidth="21600" windowHeight="11295" activeTab="7" xr2:uid="{273AC0EA-EF08-44F8-A0C8-9FE87C213ADF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="5" r:id="rId1"/>
@@ -235,10 +235,10 @@
     <t>https://www.gornphoto.com/corporate-headshots</t>
   </si>
   <si>
-    <t>RECON Restoration LLC</t>
-  </si>
-  <si>
-    <t>Damage fire repair</t>
+    <t>Creative Home Improvement LLC</t>
+  </si>
+  <si>
+    <t>windows replacement</t>
   </si>
 </sst>
 </file>
@@ -308,7 +308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -318,6 +318,8 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3732,33 +3734,37 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2">
-        <v>30.505310933327799</v>
-      </c>
-      <c r="B2">
-        <v>-84.246529702815906</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="A2" s="7">
+        <v>41.313694640000001</v>
+      </c>
+      <c r="B2" s="7">
+        <v>-73.13749971</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E2">
-        <v>50</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" s="7">
+        <v>50</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>15</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>25</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3904,18 +3910,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3937,6 +3943,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A36AE763-E731-4E22-A2A8-B95A3FB1C3CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55C74F9F-E0D3-4BAB-88E8-2452B26F1F45}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -3950,12 +3964,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A36AE763-E731-4E22-A2A8-B95A3FB1C3CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>